<commit_message>
add calculation of label
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="_56F9DC9755BA473782653E2940F9" sheetId="1" state="hidden" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t xml:space="preserve">xStJSPO0fEawe8MkOXgVH3e1f0pdtqpPhaA5DycwyupUMVkzOEk5VEdNR0NJSDVPTFdBQk1EREZNOC4u</t>
   </si>
@@ -89,6 +89,60 @@
   <si>
     <t xml:space="preserve">我可是划时代的人工智能机器人，我可是不知疲倦的在不断的学习中，学习是让人变聪明的最直接的方式，厉害吧？</t>
   </si>
+  <si>
+    <t xml:space="preserve">answer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">answer2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">answer3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfaas</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Hello</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">，晚上好</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">dasds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gfartaeerawrdaf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das</t>
+  </si>
+  <si>
+    <t xml:space="preserve">safasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fsdad</t>
+  </si>
 </sst>
 </file>
 
@@ -98,7 +152,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -127,6 +181,12 @@
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC Regular"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,7 +231,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -181,6 +241,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,10 +307,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -325,6 +389,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -341,17 +410,84 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="78.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.36"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>